<commit_message>
Add user guide sheet and fix VBA code
- Add HUONG DAN SU DUNG sheet to Excel file
- Fix UpdateWarehouseColors to use direct cell reference
- Add report button wrapper functions (BtnBaoCaoTongHop, BtnBaoCaoChiTiet)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/QuanLyKho.xlsx
+++ b/QuanLyKho.xlsx
@@ -12,6 +12,7 @@
     <sheet name="PHAT SINH" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="TON KHO" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="BAO CAO" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="HUONG DAN SU DUNG" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -246,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -307,6 +308,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3095,4 +3097,331 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="30" t="inlineStr">
+        <is>
+          <t>HUONG DAN SU DUNG - QUAN LY KHO GO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1. GIAO DIEN CHINH (Sheet SO DO KHO)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - So do kho: 104 o kho (K1-K104) xep 4 hang</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Mau sac:</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     + Trang: O mo, trong</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     + Xanh la: O mo, co hang</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     + Xam: O dong</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Vung thong tin: Hien thi thong tin o kho dang chon</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2. THAO TAC CO BAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   a) Xem thong tin o kho:</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Click vao o kho bat ky (K1-K104)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Thong tin hien thi ben phai</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   b) Nhap hang:</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Chon o kho → Nhan nut [Nhap]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Chon san pham, nhap so tam</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Nhan [Xac nhan]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   c) Xuat hang:</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Chon o kho → Nhan nut [Xuat]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Chon san pham, nhap so tam (khong vuot qua ton)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Nhan [Xac nhan]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   d) Dong/Mo o kho:</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - Chon o kho → Nhan nut [Dong] hoac [Mo]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      - O dong khong the nhap/xuat hang</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>3. QUAN LY DU LIEU</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Sheet VI TRI: Danh sach 104 vi tri, trang thai Mo/Dong</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Sheet SAN PHAM: Danh muc san pham go</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Sheet PHAT SINH: Lich su xuat/nhap (tu dong ghi)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Sheet TON KHO: Ton kho theo vi tri va san pham</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>4. BAO CAO</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Vao sheet BAO CAO</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Nhap Tu ngay (B3) va Den ngay (D3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Nhan nut [Bao cao tong hop] hoac [Bao cao chi tiet]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>5. LUU Y QUAN TRONG</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Luon luu file sau khi thao tac</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Khong xoa cac dong header trong cac sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Khong doi ten cac sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - File phai luu dang .xlsm de giu VBA code</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Bat Macros khi mo file</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>